<commit_message>
added new endpoint descriptions
</commit_message>
<xml_diff>
--- a/data/SuperEndpoint Mapping 2020SEPT18.xlsx
+++ b/data/SuperEndpoint Mapping 2020SEPT18.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://pnnl-my.sharepoint.com/personal/sara_gosline_pnnl_gov/Documents/Documents/GitHub/srpAnalytics/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="7" documentId="13_ncr:1_{F702D4E1-403C-442A-AAFF-4D64E98CB541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{49F02887-D40A-4519-B248-19C7D550F07F}"/>
+  <xr:revisionPtr revIDLastSave="23" documentId="13_ncr:1_{F702D4E1-403C-442A-AAFF-4D64E98CB541}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A509F0A5-D35A-4BE8-8E76-5D9AC9EA4BEC}"/>
   <bookViews>
-    <workbookView xWindow="7305" yWindow="4380" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Original" sheetId="4" r:id="rId1"/>
@@ -244,12 +244,6 @@
     <t>Total mortality</t>
   </si>
   <si>
-    <t>Any effect 24hr</t>
-  </si>
-  <si>
-    <t>Any except mort</t>
-  </si>
-  <si>
     <t>Total mortality (aggregation of MO24 + MORT)</t>
   </si>
   <si>
@@ -593,24 +587,6 @@
   </si>
   <si>
     <t>Lac of spontaneous motion at 24hrs</t>
-  </si>
-  <si>
-    <t>Sp Motion at 24h</t>
-  </si>
-  <si>
-    <t>Any effect by 5 d</t>
-  </si>
-  <si>
-    <t>Notochord at 5d</t>
-  </si>
-  <si>
-    <t>Delay dev prog 24h</t>
-  </si>
-  <si>
-    <t>5d behavior trans</t>
-  </si>
-  <si>
-    <t>5d behavior total</t>
   </si>
   <si>
     <r>
@@ -690,6 +666,30 @@
   </si>
   <si>
     <t>http://purl.obolibrary.org/obo/ZP_0015467</t>
+  </si>
+  <si>
+    <t>Any effect in 5 days</t>
+  </si>
+  <si>
+    <t>Any effect except mortality</t>
+  </si>
+  <si>
+    <t>5 day behavior transition</t>
+  </si>
+  <si>
+    <t>Notochord at 5 days</t>
+  </si>
+  <si>
+    <t>Spontaneous motion at 24h</t>
+  </si>
+  <si>
+    <t>Delayed development at 24h</t>
+  </si>
+  <si>
+    <t>5 day total movement</t>
+  </si>
+  <si>
+    <t>Any effect in 24 hours</t>
   </si>
 </sst>
 </file>
@@ -1187,13 +1187,13 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="C1" t="s">
         <v>69</v>
       </c>
       <c r="F1" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
@@ -1201,10 +1201,10 @@
         <v>7</v>
       </c>
       <c r="B2" t="s">
+        <v>84</v>
+      </c>
+      <c r="C2" t="s">
         <v>86</v>
-      </c>
-      <c r="C2" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -1212,10 +1212,10 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C3" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -1223,10 +1223,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C4" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -1234,21 +1234,21 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C5" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B6" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C6" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -1256,21 +1256,21 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C7" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B8" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C8" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -1278,10 +1278,10 @@
         <v>26</v>
       </c>
       <c r="B9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C9" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -1289,43 +1289,43 @@
         <v>29</v>
       </c>
       <c r="B10" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="C10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C11" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B12" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C12" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B13" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C13" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -1333,10 +1333,10 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="C14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -1344,43 +1344,43 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C15" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B16" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C16" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B17" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C17" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B18" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C18" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1388,43 +1388,43 @@
         <v>30</v>
       </c>
       <c r="B19" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C19" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C20" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B21" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C21" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B22" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C22" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
     </row>
   </sheetData>
@@ -1745,96 +1745,96 @@
   <dimension ref="A1:E21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="13.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
-    <col min="3" max="3" width="19.7109375" customWidth="1"/>
+    <col min="3" max="3" width="27" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="74.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>195</v>
+        <v>187</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D1" t="s">
         <v>69</v>
       </c>
       <c r="E1" t="s">
-        <v>198</v>
+        <v>190</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B2" s="8" t="s">
         <v>59</v>
       </c>
       <c r="C2" t="s">
-        <v>72</v>
+        <v>206</v>
       </c>
       <c r="D2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>57</v>
       </c>
       <c r="C3" t="s">
-        <v>189</v>
+        <v>205</v>
       </c>
       <c r="D3" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>56</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>212</v>
       </c>
       <c r="D4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B5" s="8" t="s">
         <v>68</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>193</v>
+        <v>211</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="E5" t="s">
-        <v>199</v>
+        <v>191</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B6" s="8" t="s">
         <v>9</v>
@@ -1843,15 +1843,15 @@
         <v>8</v>
       </c>
       <c r="D6" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="E6" t="s">
-        <v>200</v>
+        <v>192</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B7" s="8" t="s">
         <v>60</v>
@@ -1860,15 +1860,15 @@
         <v>10</v>
       </c>
       <c r="D7" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="E7" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B8" s="8" t="s">
         <v>61</v>
@@ -1877,32 +1877,32 @@
         <v>14</v>
       </c>
       <c r="D8" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="E8" t="s">
-        <v>202</v>
+        <v>194</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B9" s="8" t="s">
         <v>4</v>
       </c>
       <c r="C9" t="s">
-        <v>191</v>
+        <v>210</v>
       </c>
       <c r="D9" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E9" t="s">
-        <v>203</v>
+        <v>195</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B10" s="8" t="s">
         <v>62</v>
@@ -1911,15 +1911,15 @@
         <v>19</v>
       </c>
       <c r="D10" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="E10" s="13" t="s">
-        <v>204</v>
+        <v>196</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B11" s="8" t="s">
         <v>63</v>
@@ -1928,32 +1928,32 @@
         <v>23</v>
       </c>
       <c r="D11" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="E11" t="s">
-        <v>205</v>
+        <v>197</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B12" s="8" t="s">
         <v>3</v>
       </c>
       <c r="C12" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E12" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B13" s="8" t="s">
         <v>7</v>
@@ -1962,32 +1962,32 @@
         <v>43</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="E13" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B14" s="8" t="s">
         <v>67</v>
       </c>
       <c r="C14" s="10" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="E14" t="s">
-        <v>207</v>
+        <v>199</v>
       </c>
     </row>
     <row r="15" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B15" s="8" t="s">
         <v>64</v>
@@ -1996,49 +1996,49 @@
         <v>27</v>
       </c>
       <c r="D15" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="E15" t="s">
-        <v>208</v>
+        <v>200</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B16" s="8" t="s">
         <v>39</v>
       </c>
       <c r="C16" t="s">
-        <v>190</v>
+        <v>208</v>
       </c>
       <c r="D16" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="E16" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B17" s="11" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="C17" s="12" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="D17" s="12" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="E17" t="s">
-        <v>209</v>
+        <v>201</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B18" s="8" t="s">
         <v>65</v>
@@ -2047,32 +2047,32 @@
         <v>32</v>
       </c>
       <c r="D18" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E18" t="s">
-        <v>210</v>
+        <v>202</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B19" s="8" t="s">
         <v>5</v>
       </c>
       <c r="C19" s="10" t="s">
-        <v>188</v>
+        <v>209</v>
       </c>
       <c r="D19" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="E19" t="s">
-        <v>211</v>
+        <v>203</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>197</v>
+        <v>189</v>
       </c>
       <c r="B20" s="8" t="s">
         <v>66</v>
@@ -2081,15 +2081,15 @@
         <v>35</v>
       </c>
       <c r="D20" t="s">
-        <v>194</v>
+        <v>186</v>
       </c>
       <c r="E20" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>196</v>
+        <v>188</v>
       </c>
       <c r="B21" s="8" t="s">
         <v>58</v>
@@ -2098,10 +2098,10 @@
         <v>70</v>
       </c>
       <c r="D21" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="E21" t="s">
-        <v>206</v>
+        <v>198</v>
       </c>
     </row>
   </sheetData>
@@ -2135,35 +2135,35 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
       <c r="B1" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="C1" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B2" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C3" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
@@ -2171,10 +2171,10 @@
         <v>26</v>
       </c>
       <c r="B4" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="C4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -2182,43 +2182,43 @@
         <v>29</v>
       </c>
       <c r="B5" t="s">
-        <v>150</v>
+        <v>148</v>
       </c>
       <c r="C5" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B6" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="C6" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="B7" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C7" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B8" t="s">
-        <v>156</v>
+        <v>154</v>
       </c>
       <c r="C8" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -2226,7 +2226,7 @@
         <v>12</v>
       </c>
       <c r="B9" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -2234,43 +2234,43 @@
         <v>13</v>
       </c>
       <c r="B10" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C10" t="s">
-        <v>158</v>
+        <v>156</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B11" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="C11" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B12" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C12" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="B13" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C13" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -2278,52 +2278,52 @@
         <v>30</v>
       </c>
       <c r="B14" t="s">
+        <v>158</v>
+      </c>
+      <c r="C14" t="s">
+        <v>159</v>
+      </c>
+      <c r="E14" t="s">
         <v>160</v>
       </c>
-      <c r="C14" t="s">
+      <c r="F14" t="s">
         <v>161</v>
       </c>
-      <c r="E14" t="s">
+      <c r="G14" t="s">
         <v>162</v>
-      </c>
-      <c r="F14" t="s">
-        <v>163</v>
-      </c>
-      <c r="G14" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B15" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C15" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B16" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C16" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B17" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C17" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
@@ -2331,38 +2331,38 @@
         <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="C18" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
+        <v>166</v>
+      </c>
+      <c r="B19" t="s">
+        <v>167</v>
+      </c>
+      <c r="C19" t="s">
         <v>168</v>
       </c>
-      <c r="B19" t="s">
-        <v>169</v>
-      </c>
-      <c r="C19" t="s">
-        <v>170</v>
-      </c>
       <c r="E19" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="B20" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C20" t="s">
+        <v>170</v>
+      </c>
+      <c r="E20" t="s">
         <v>172</v>
-      </c>
-      <c r="E20" t="s">
-        <v>174</v>
       </c>
     </row>
   </sheetData>
@@ -2371,6 +2371,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100396ED2E7A640164CB8C59FDEC2C765CC" ma:contentTypeVersion="8" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="26e8590940edae28bea0b080f6fa8b06">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="aceb4bc4-7be6-4130-8e8a-7008d72bfcc3" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="7a9331905dac936d9e88b896f6b901d6" ns3:_="">
     <xsd:import namespace="aceb4bc4-7be6-4130-8e8a-7008d72bfcc3"/>
@@ -2540,35 +2555,10 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8D080FC-E009-4447-ACD6-B9CB0ED3D7DD}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E57FCB-AF0B-40B5-9F88-8BBFA3B90FEE}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="aceb4bc4-7be6-4130-8e8a-7008d72bfcc3"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -2590,9 +2580,19 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{49E57FCB-AF0B-40B5-9F88-8BBFA3B90FEE}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{E8D080FC-E009-4447-ACD6-B9CB0ED3D7DD}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="aceb4bc4-7be6-4130-8e8a-7008d72bfcc3"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>